<commit_message>
Work Schedule Update 24
Work Schedule Update 24
</commit_message>
<xml_diff>
--- a/Civilworks cost/Work Schedule/Kishoregonj Packages/finalestimate_kishoregonjprotectivework/Flood Fuse -14_12.10.2020/Flood Fuse -14_12.10.2020/Pac-34/Schdule Input.xlsx
+++ b/Civilworks cost/Work Schedule/Kishoregonj Packages/finalestimate_kishoregonjprotectivework/Flood Fuse -14_12.10.2020/Flood Fuse -14_12.10.2020/Pac-34/Schdule Input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="10" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="11" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Resource_List" sheetId="19" r:id="rId1"/>
@@ -1180,12 +1180,12 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1355,11 +1355,11 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1625,15 +1625,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="I15" sqref="I15:I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="47.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2142,11 +2142,11 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="47.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2589,11 +2589,11 @@
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="47.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2977,15 +2977,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="47.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3210,12 +3210,12 @@
       <selection activeCell="G1" sqref="G1:G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="47.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3392,11 +3392,11 @@
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="47.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3573,11 +3573,11 @@
       <selection activeCell="G1" sqref="G1:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="47.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3708,11 +3708,11 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="47.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3843,15 +3843,15 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1"/>
-    <col min="2" max="2" width="52.44140625" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" customWidth="1"/>
-    <col min="9" max="9" width="42.6640625" customWidth="1"/>
-    <col min="10" max="10" width="47.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="52.42578125" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="42.7109375" customWidth="1"/>
+    <col min="10" max="10" width="47.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -4354,16 +4354,16 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" customWidth="1"/>
-    <col min="5" max="6" width="13.6640625" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" customWidth="1"/>
-    <col min="8" max="8" width="13.44140625" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -5485,15 +5485,15 @@
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="4.5546875" customWidth="1"/>
-    <col min="3" max="4" width="4.88671875" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" customWidth="1"/>
+    <col min="3" max="4" width="4.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="15" customFormat="1" ht="42" customHeight="1">
@@ -5896,11 +5896,11 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="56.33203125" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="1"/>
+    <col min="1" max="1" width="56.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -6003,7 +6003,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6017,10 +6017,10 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -6162,13 +6162,13 @@
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -6355,11 +6355,11 @@
       <selection activeCell="A14" sqref="A14:E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="32.109375" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" customWidth="1"/>
-    <col min="4" max="4" width="38.33203125" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" customWidth="1"/>
     <col min="5" max="5" width="65" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6414,7 +6414,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.8">
+    <row r="4" spans="1:5" ht="45">
       <c r="A4" s="3" t="s">
         <v>118</v>
       </c>
@@ -6431,7 +6431,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.8">
+    <row r="5" spans="1:5" ht="30">
       <c r="A5" s="3" t="s">
         <v>120</v>
       </c>
@@ -6448,7 +6448,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="28.8">
+    <row r="6" spans="1:5" ht="30">
       <c r="A6" s="6" t="s">
         <v>129</v>
       </c>
@@ -6465,7 +6465,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="28.8">
+    <row r="7" spans="1:5" ht="30">
       <c r="A7" s="3" t="s">
         <v>131</v>
       </c>
@@ -6482,7 +6482,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28.8">
+    <row r="8" spans="1:5" ht="30">
       <c r="A8" s="3" t="s">
         <v>133</v>
       </c>
@@ -6499,7 +6499,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="28.8">
+    <row r="9" spans="1:5" ht="30">
       <c r="A9" s="3" t="s">
         <v>135</v>
       </c>
@@ -6516,7 +6516,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="28.8">
+    <row r="10" spans="1:5" ht="45">
       <c r="A10" s="3" t="s">
         <v>137</v>
       </c>
@@ -6533,7 +6533,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28.8">
+    <row r="11" spans="1:5" ht="45">
       <c r="A11" s="3" t="s">
         <v>139</v>
       </c>
@@ -6550,7 +6550,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="28.8">
+    <row r="12" spans="1:5" ht="30">
       <c r="A12" s="49" t="s">
         <v>144</v>
       </c>
@@ -6567,7 +6567,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="28.8">
+    <row r="13" spans="1:5" ht="30">
       <c r="A13" s="49" t="s">
         <v>146</v>
       </c>
@@ -6584,7 +6584,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="28.8">
+    <row r="14" spans="1:5" ht="30">
       <c r="A14" s="5" t="s">
         <v>147</v>
       </c>
@@ -6618,13 +6618,13 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -6897,11 +6897,11 @@
       <selection activeCell="A2" sqref="A2:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -7171,11 +7171,11 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">

</xml_diff>